<commit_message>
Models Updated, Javascript halfway done, routes halfwaydone, css improved.
</commit_message>
<xml_diff>
--- a/Tables_Structure_Pseudo_Code.xlsx
+++ b/Tables_Structure_Pseudo_Code.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wcali\OneDrive\Desktop\project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/242df245c821da1d/Desktop/project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F74756-061D-47E7-B61E-4B03DAB37297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{20F74756-061D-47E7-B61E-4B03DAB37297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB0EFE81-2381-4865-B262-096E92A742D1}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0815AA7F-E934-455B-ACC7-EAD78B28A99B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Morning</t>
   </si>
@@ -77,18 +77,12 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Calendar</t>
-  </si>
-  <si>
     <t>StarbucKs</t>
   </si>
   <si>
     <t>Restaurant</t>
   </si>
   <si>
-    <t>etc</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -98,30 +92,12 @@
     <t>Harris</t>
   </si>
   <si>
-    <t>Pearland</t>
-  </si>
-  <si>
-    <t>Downtown</t>
-  </si>
-  <si>
-    <t>Event Request</t>
-  </si>
-  <si>
-    <t>Atendees</t>
-  </si>
-  <si>
-    <t>Interests (Array of Event Foreign keys)</t>
-  </si>
-  <si>
     <t>Have a coffe</t>
   </si>
   <si>
     <t>Interest</t>
   </si>
   <si>
-    <t>Chace, Kiki</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -132,6 +108,27 @@
   </si>
   <si>
     <t>Interest ID (Foreign Key)</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Event ID (Foreign Key)</t>
+  </si>
+  <si>
+    <t>Username (Foreign Key)</t>
+  </si>
+  <si>
+    <t>User Interest</t>
+  </si>
+  <si>
+    <t>Hang Out</t>
+  </si>
+  <si>
+    <t>Hangout Members</t>
+  </si>
+  <si>
+    <t>ate</t>
   </si>
 </sst>
 </file>
@@ -139,7 +136,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -270,13 +267,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,51 +605,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0974601-002C-4583-A6E1-49FC9C3E99F9}">
-  <dimension ref="A3:P11"/>
+  <dimension ref="A3:Q19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="78" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="3.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.20703125" customWidth="1"/>
-    <col min="4" max="4" width="30.1015625" customWidth="1"/>
-    <col min="5" max="5" width="5.1015625" customWidth="1"/>
-    <col min="6" max="6" width="7.734375" customWidth="1"/>
-    <col min="7" max="7" width="25.1015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.41796875" customWidth="1"/>
-    <col min="9" max="9" width="3.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.734375" customWidth="1"/>
-    <col min="11" max="11" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.9453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.3125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.83984375" customWidth="1"/>
+    <col min="2" max="2" width="14.41796875" customWidth="1"/>
+    <col min="3" max="3" width="15.62890625" customWidth="1"/>
+    <col min="4" max="4" width="13.734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5234375" customWidth="1"/>
+    <col min="6" max="6" width="5.1015625" customWidth="1"/>
+    <col min="7" max="7" width="8.47265625" customWidth="1"/>
+    <col min="8" max="8" width="34.15625" customWidth="1"/>
+    <col min="9" max="9" width="22.3671875" customWidth="1"/>
+    <col min="10" max="10" width="3.89453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.734375" customWidth="1"/>
+    <col min="12" max="12" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.9453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="34.578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.3125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="4" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="5" spans="1:16" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="4" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="5" spans="1:17" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -660,212 +657,277 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="7" spans="1:16" ht="46.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:17" ht="46.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="D7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="G7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="K7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="13" t="s">
+      <c r="P7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="1"/>
-      <c r="F8" s="3">
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="K8" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="4">
         <v>43925</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>2</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="4">
+      <c r="N9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="4">
         <v>43925</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="1:16" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="3"/>
-      <c r="F10" s="3">
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="G10" s="3">
         <v>3</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3">
-        <v>3</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" s="6">
-        <v>43927</v>
-      </c>
-      <c r="O10" s="3" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="2">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="2"/>
-      <c r="F11" s="2">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="G11" s="2">
         <v>4</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="10"/>
+      <c r="Q12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="G13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="Q14" s="10"/>
+    </row>
+    <row r="15" spans="1:17" ht="93.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="10"/>
+    </row>
+    <row r="16" spans="1:17" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="8"/>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="9"/>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="8"/>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="2">
         <v>4</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="5">
-        <v>43928</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="9"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="9"/>
+      <c r="G19" s="2">
+        <v>4</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="9"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8:L11" xr:uid="{EB5DD3E4-08AF-49A9-BEDF-012C8AA51E4A}">
-      <formula1>$G$8:$G$11</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8:M11" xr:uid="{EB5DD3E4-08AF-49A9-BEDF-012C8AA51E4A}">
+      <formula1>$H$8:$H$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J8:J11" xr:uid="{BF074EF0-474C-404F-8C9E-A14960368235}">
-      <formula1>$B$8:$B$11</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K11" xr:uid="{BF074EF0-474C-404F-8C9E-A14960368235}">
+      <formula1>$C$8:$C$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding a basic readme file and updating the presentation.
</commit_message>
<xml_diff>
--- a/Tables_Structure_Pseudo_Code.xlsx
+++ b/Tables_Structure_Pseudo_Code.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/242df245c821da1d/Desktop/project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{20F74756-061D-47E7-B61E-4B03DAB37297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB0EFE81-2381-4865-B262-096E92A742D1}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{20F74756-061D-47E7-B61E-4B03DAB37297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4DE932BD-5EF5-4C5D-B34C-52434815ABB1}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0815AA7F-E934-455B-ACC7-EAD78B28A99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$18:$F$21</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Morning</t>
   </si>
@@ -44,15 +47,9 @@
     <t>Dinner</t>
   </si>
   <si>
-    <t>Play Soccer</t>
-  </si>
-  <si>
     <t>Go to Museum</t>
   </si>
   <si>
-    <t>Talk About Politics</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -74,30 +71,9 @@
     <t>User</t>
   </si>
   <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>StarbucKs</t>
-  </si>
-  <si>
-    <t>Restaurant</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Event Comment</t>
-  </si>
-  <si>
     <t>Harris</t>
   </si>
   <si>
-    <t>Have a coffe</t>
-  </si>
-  <si>
-    <t>Interest</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -107,28 +83,49 @@
     <t>User ID (Foregin Key)</t>
   </si>
   <si>
-    <t>Interest ID (Foreign Key)</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Event ID (Foreign Key)</t>
-  </si>
-  <si>
-    <t>Username (Foreign Key)</t>
-  </si>
-  <si>
-    <t>User Interest</t>
-  </si>
-  <si>
     <t>Hang Out</t>
   </si>
   <si>
-    <t>Hangout Members</t>
-  </si>
-  <si>
-    <t>ate</t>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Hangout Input</t>
+  </si>
+  <si>
+    <t>Hangout Comments</t>
+  </si>
+  <si>
+    <t>Atendeed</t>
+  </si>
+  <si>
+    <t>chace@gmail.com</t>
+  </si>
+  <si>
+    <t>ike@gmail.com</t>
+  </si>
+  <si>
+    <t>kiki@gmail.com</t>
+  </si>
+  <si>
+    <t>wilson@gmail.com</t>
+  </si>
+  <si>
+    <t>Have a coffee at Stabucks</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Going to a museum this afternoon</t>
+  </si>
+  <si>
+    <t>Having a coffe at Starbucks.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -252,11 +249,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -289,6 +299,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -605,30 +621,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0974601-002C-4583-A6E1-49FC9C3E99F9}">
-  <dimension ref="A3:Q19"/>
+  <dimension ref="A3:S27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="A5:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.41796875" customWidth="1"/>
-    <col min="3" max="3" width="15.62890625" customWidth="1"/>
-    <col min="4" max="4" width="13.734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5234375" customWidth="1"/>
-    <col min="6" max="6" width="5.1015625" customWidth="1"/>
-    <col min="7" max="7" width="8.47265625" customWidth="1"/>
-    <col min="8" max="8" width="34.15625" customWidth="1"/>
-    <col min="9" max="9" width="22.3671875" customWidth="1"/>
-    <col min="10" max="10" width="3.89453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.734375" customWidth="1"/>
-    <col min="12" max="12" width="15.41796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.9453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.3125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.578125" customWidth="1"/>
+    <col min="3" max="3" width="31.26171875" customWidth="1"/>
+    <col min="4" max="4" width="29.68359375" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="33.9453125" customWidth="1"/>
+    <col min="7" max="7" width="35.3671875" customWidth="1"/>
+    <col min="8" max="8" width="30.578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.9453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="38.5234375" customWidth="1"/>
+    <col min="13" max="13" width="15.3671875" customWidth="1"/>
+    <col min="14" max="14" width="19.734375" customWidth="1"/>
     <col min="15" max="15" width="34.578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.3125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="14.3125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.83984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -636,68 +652,32 @@
     <row r="4" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="5" spans="1:17" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A5" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
+      <c r="G5" s="12"/>
       <c r="P5" s="12"/>
     </row>
     <row r="6" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="7" spans="1:17" ht="46.5" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E7" s="10"/>
-      <c r="G7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>31</v>
-      </c>
       <c r="P7" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="10"/>
     </row>
@@ -705,129 +685,73 @@
       <c r="A8" s="1">
         <v>1</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="8">
+        <v>123</v>
+      </c>
       <c r="E8" s="10"/>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" s="4">
-        <v>43925</v>
-      </c>
       <c r="P8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:17" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="D9" s="9">
+        <v>123</v>
+      </c>
       <c r="E9" s="10"/>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O9" s="4">
-        <v>43925</v>
-      </c>
       <c r="P9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:17" ht="18.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="3">
         <v>3</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="D10" s="8">
+        <v>123</v>
+      </c>
       <c r="E10" s="10"/>
-      <c r="G10" s="3">
-        <v>3</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="6"/>
       <c r="P10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:17" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="2">
         <v>4</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="D11" s="9">
+        <v>123</v>
+      </c>
       <c r="E11" s="10"/>
-      <c r="G11" s="2">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="5"/>
       <c r="P11" s="2" t="s">
         <v>2</v>
       </c>
@@ -837,99 +761,138 @@
       <c r="E12" s="10"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="G13" s="11" t="s">
+    <row r="15" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="46.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="46.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:17" ht="20.399999999999999" x14ac:dyDescent="0.75">
-      <c r="A14" s="11"/>
-      <c r="E14" s="10"/>
-      <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" ht="93.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="13" t="s">
+      <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>43925</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="46.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" ht="23.7" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="8"/>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="2">
+      <c r="D19" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="9"/>
-      <c r="G17" s="2">
-        <v>2</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="3">
+      <c r="G19" s="4">
+        <v>43925</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="8"/>
-      <c r="G18" s="3">
-        <v>3</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="23.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="9"/>
-      <c r="G19" s="2">
-        <v>4</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="9"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="D27" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8:M11" xr:uid="{EB5DD3E4-08AF-49A9-BEDF-012C8AA51E4A}">
-      <formula1>$H$8:$H$11</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K11" xr:uid="{BF074EF0-474C-404F-8C9E-A14960368235}">
-      <formula1>$C$8:$C$11</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>